<commit_message>
Feat: design schema database v1.2 - normalisasi phase 1
</commit_message>
<xml_diff>
--- a/concept/normalisasi-keuangan.xlsx
+++ b/concept/normalisasi-keuangan.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17960" activeTab="1"/>
+    <workbookView windowHeight="18560" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="unnormal" sheetId="1" r:id="rId1"/>
     <sheet name="1nf" sheetId="2" r:id="rId2"/>
     <sheet name="2nf" sheetId="3" r:id="rId3"/>
+    <sheet name="3nf" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="47">
   <si>
     <t>Tanggal Proses</t>
   </si>
@@ -127,25 +128,49 @@
     <t>email</t>
   </si>
   <si>
+    <t>email_verified_at</t>
+  </si>
+  <si>
+    <t>remember_token</t>
+  </si>
+  <si>
+    <t>asep@gmail.com</t>
+  </si>
+  <si>
+    <t>feby@gmail.com</t>
+  </si>
+  <si>
+    <t>Kategori (Tipe)</t>
+  </si>
+  <si>
+    <t>pencatat</t>
+  </si>
+  <si>
+    <t>id_kategori</t>
+  </si>
+  <si>
+    <t>id_sub_kategori</t>
+  </si>
+  <si>
+    <t>Sub Kategori (Kategori)</t>
+  </si>
+  <si>
+    <t>id_role</t>
+  </si>
+  <si>
     <t>role</t>
   </si>
   <si>
-    <t>email_verified_at</t>
-  </si>
-  <si>
-    <t>remember_token</t>
-  </si>
-  <si>
-    <t>asep@gmail.com</t>
-  </si>
-  <si>
     <t>administrator</t>
   </si>
   <si>
-    <t>feby@gmail.com</t>
-  </si>
-  <si>
     <t>manager</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>deskripsi</t>
   </si>
 </sst>
 </file>
@@ -161,10 +186,17 @@
     <numFmt numFmtId="177" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??.00_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="0.0000_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -314,12 +346,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.25"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -634,73 +696,58 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -709,62 +756,77 @@
     <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -774,26 +836,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -1073,6 +1174,49 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>322580</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Screenshot 2025-05-07 at 19.33.08"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="754380" y="426720"/>
+          <a:ext cx="14198600" cy="8667750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -1334,7 +1478,7 @@
   <dimension ref="C5:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H10"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -1342,9 +1486,9 @@
     <col min="3" max="3" width="22" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
     <col min="5" max="5" width="11.59375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.40625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21.8671875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="38.796875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16.40625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="21.8671875" style="19" customWidth="1"/>
+    <col min="8" max="8" width="38.796875" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:8">
@@ -1357,18 +1501,18 @@
       <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="3:8">
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>45771</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1377,18 +1521,18 @@
       <c r="E6" s="1">
         <v>1500000</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="3:8">
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>45772</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1397,18 +1541,18 @@
       <c r="E7" s="1">
         <v>200000</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="3:8">
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>45772</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1417,18 +1561,18 @@
       <c r="E8" s="1">
         <v>100000</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="3:8">
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>45772</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1437,18 +1581,18 @@
       <c r="E9" s="1">
         <v>100000</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="3:8">
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>45772</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1457,13 +1601,13 @@
       <c r="E10" s="1">
         <v>100000</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="19" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1478,8 +1622,8 @@
   <sheetPr/>
   <dimension ref="B4:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1535,7 +1679,7 @@
       <c r="B6" s="1">
         <v>22</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>45771</v>
       </c>
       <c r="D6" s="1">
@@ -1547,10 +1691,10 @@
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="20" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1558,7 +1702,7 @@
       <c r="B7" s="1">
         <v>11</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>45772</v>
       </c>
       <c r="D7" s="1">
@@ -1570,10 +1714,10 @@
       <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="20" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1581,7 +1725,7 @@
       <c r="B8" s="1">
         <v>12</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>45772</v>
       </c>
       <c r="D8" s="1">
@@ -1593,10 +1737,10 @@
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1604,7 +1748,7 @@
       <c r="B9" s="1">
         <v>10</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>45772</v>
       </c>
       <c r="D9" s="1">
@@ -1616,10 +1760,10 @@
       <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="20" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1627,7 +1771,7 @@
       <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>45772</v>
       </c>
       <c r="D10" s="1">
@@ -1639,10 +1783,10 @@
       <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1651,7 +1795,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" ht="17" spans="2:10">
+    <row r="15" ht="17" spans="2:9">
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1664,19 +1808,16 @@
       <c r="E15" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" t="s">
         <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="I15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1690,12 +1831,10 @@
       <c r="D16" s="1">
         <v>123</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E16" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="1">
@@ -1707,20 +1846,18 @@
       <c r="D17" s="1">
         <v>123</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="E17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="1"/>
     </row>
     <row r="25" spans="7:8">
-      <c r="G25" s="6"/>
-      <c r="H25" s="9"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="21"/>
     </row>
     <row r="26" spans="7:8">
-      <c r="G26" s="7"/>
-      <c r="H26" s="10"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1735,10 +1872,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B4:R26"/>
+  <dimension ref="B4:S28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1748,210 +1885,294 @@
     <col min="4" max="4" width="18.09375" customWidth="1"/>
     <col min="5" max="6" width="15.234375" customWidth="1"/>
     <col min="7" max="7" width="17.4453125" customWidth="1"/>
-    <col min="8" max="8" width="27.2109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.9765625" customWidth="1"/>
-    <col min="10" max="10" width="14.1875" customWidth="1"/>
+    <col min="10" max="10" width="20.1796875" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" customWidth="1"/>
     <col min="15" max="15" width="9" style="1"/>
     <col min="16" max="16" width="12.2421875" customWidth="1"/>
     <col min="17" max="17" width="11.9765625" customWidth="1"/>
     <col min="18" max="18" width="13.8046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:16">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" ht="17" spans="2:18">
-      <c r="B5" s="1" t="s">
+      <c r="H4"/>
+      <c r="I4" s="2"/>
+      <c r="O4"/>
+      <c r="P4" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" ht="17" spans="2:19">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5"/>
+      <c r="P5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="Q5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="R5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K5" t="s">
+      <c r="S5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>25</v>
-      </c>
-      <c r="R5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" ht="51" spans="2:16">
+    </row>
+    <row r="6" ht="34" spans="2:17">
       <c r="B6" s="1">
         <v>22</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>45771</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
         <v>1500000</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="K6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6"/>
+      <c r="P6" s="1">
         <v>1</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" ht="17" spans="2:16">
+    <row r="7" ht="34" spans="2:17">
       <c r="B7" s="1">
         <v>11</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
         <v>45772</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
         <v>200000</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>2</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="K7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7"/>
+      <c r="P7" s="1">
         <v>2</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="17" spans="2:9">
+    <row r="8" ht="17" spans="2:16">
       <c r="B8" s="1">
         <v>12</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>45772</v>
       </c>
       <c r="D8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1">
         <v>100000</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>2</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+      <c r="J8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="K8" s="20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" ht="17" spans="2:9">
+      <c r="O8"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" ht="17" spans="2:16">
       <c r="B9" s="1">
         <v>10</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>45772</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1">
         <v>100000</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>2</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="K9" s="20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" ht="17" spans="2:9">
+      <c r="O9"/>
+      <c r="P9" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" ht="17" spans="2:19">
       <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <v>45772</v>
       </c>
       <c r="D10" s="1">
         <v>2</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1">
         <v>100000</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>2</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="2">
+        <v>2</v>
+      </c>
+      <c r="J10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="K10" s="20" t="s">
         <v>16</v>
+      </c>
+      <c r="O10"/>
+      <c r="P10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="S10" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="8:17">
+      <c r="H11"/>
+      <c r="I11" s="2"/>
+      <c r="O11"/>
+      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="8:17">
+      <c r="H12"/>
+      <c r="I12" s="2"/>
+      <c r="O12"/>
+      <c r="P12" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:2">
@@ -1959,36 +2180,39 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" ht="17" spans="2:10">
-      <c r="B15" s="1" t="s">
+    <row r="15" ht="17" spans="2:11">
+      <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="I15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="J15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:7">
       <c r="B16" s="1">
         <v>1</v>
       </c>
@@ -1998,16 +2222,17 @@
       <c r="D16" s="1">
         <v>123</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="E16" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
       <c r="B17" s="1">
         <v>2</v>
       </c>
@@ -2017,26 +2242,59 @@
       <c r="D17" s="1">
         <v>123</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17"/>
+      <c r="E17" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="18" spans="7:8">
       <c r="G18" s="2"/>
       <c r="H18"/>
     </row>
-    <row r="25" spans="8:9">
-      <c r="H25" s="6"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="8:9">
-      <c r="H26" s="7"/>
-      <c r="I26" s="10"/>
+    <row r="25" spans="5:9">
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="14"/>
+      <c r="I25" s="21"/>
+    </row>
+    <row r="26" spans="5:9">
+      <c r="E26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="5:6">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="5:6">
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2046,4 +2304,21 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>